<commit_message>
maked good sensors with green
</commit_message>
<xml_diff>
--- a/Documentation/i2c.xlsx
+++ b/Documentation/i2c.xlsx
@@ -304,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -331,11 +337,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -641,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +707,7 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3">
@@ -723,6 +730,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
       <c r="E4" t="s">
         <v>64</v>
       </c>
@@ -737,7 +745,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5">
@@ -806,7 +814,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -855,7 +863,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10">
@@ -878,7 +886,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11">
@@ -901,7 +909,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C12">
@@ -921,7 +929,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C13">

</xml_diff>